<commit_message>
Ultimate le correzioni del Pdp (si spera)
Pronto per la verifica
</commit_message>
<xml_diff>
--- a/Piano di Progetto/Preventivo - Rp.xlsx
+++ b/Piano di Progetto/Preventivo - Rp.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="42">
   <si>
     <t>Responsabile</t>
   </si>
@@ -125,6 +125,24 @@
   </si>
   <si>
     <t>pian2</t>
+  </si>
+  <si>
+    <t>Progettazione Architetturale</t>
+  </si>
+  <si>
+    <t>Progettazione di Dettaglio e Codifica</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>Costo1</t>
+  </si>
+  <si>
+    <t>Costo2</t>
+  </si>
+  <si>
+    <t>diff</t>
   </si>
 </sst>
 </file>
@@ -264,6 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -276,7 +295,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -344,7 +362,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="3.0555555555555582E-2"/>
-                  <c:y val="2.7777777777777891E-2"/>
+                  <c:y val="2.7777777777777901E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -357,8 +375,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.21111111111111117"/>
-                  <c:y val="-6.4814814814814839E-2"/>
+                  <c:x val="0.21111111111111122"/>
+                  <c:y val="-6.4814814814814853E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -434,13 +452,13 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>111</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,7 +471,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -463,7 +481,9 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="it-IT"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -523,24 +543,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="107906560"/>
-        <c:axId val="107908096"/>
+        <c:axId val="75470720"/>
+        <c:axId val="75472256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107906560"/>
+        <c:axId val="75470720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107908096"/>
+        <c:crossAx val="75472256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107908096"/>
+        <c:axId val="75472256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -548,7 +568,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107906560"/>
+        <c:crossAx val="75470720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="150"/>
@@ -558,7 +578,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -586,10 +606,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Progettazione</c:v>
+                  <c:v>Progettazione Architetturale</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Codifica</c:v>
+                  <c:v>Progettazione di Dettaglio e Codifica</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Verifica e Validazione</c:v>
@@ -604,10 +624,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5417</c:v>
+                  <c:v>4535</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4125</c:v>
+                  <c:v>4943</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2176</c:v>
@@ -637,7 +657,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -748,24 +768,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="108070400"/>
-        <c:axId val="108071936"/>
+        <c:axId val="107743104"/>
+        <c:axId val="107744640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108070400"/>
+        <c:axId val="107743104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108071936"/>
+        <c:crossAx val="107744640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108071936"/>
+        <c:axId val="107744640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -773,7 +793,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108070400"/>
+        <c:crossAx val="107743104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -786,7 +806,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -846,10 +866,10 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>111</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -916,24 +936,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="79971072"/>
-        <c:axId val="79972608"/>
+        <c:axId val="75714560"/>
+        <c:axId val="75716096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79971072"/>
+        <c:axId val="75714560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79972608"/>
+        <c:crossAx val="75716096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79972608"/>
+        <c:axId val="75716096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,7 +961,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79971072"/>
+        <c:crossAx val="75714560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -954,7 +974,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -970,10 +990,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.22371062992125984"/>
+          <c:x val="0.22371062992125981"/>
           <c:y val="5.0925925925925923E-2"/>
-          <c:w val="0.49754768153980755"/>
-          <c:h val="0.83309419655876349"/>
+          <c:w val="0.49754768153980766"/>
+          <c:h val="0.83309419655876371"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1021,19 +1041,19 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>71</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1106,24 +1126,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="90800512"/>
-        <c:axId val="90802048"/>
+        <c:axId val="75748864"/>
+        <c:axId val="75750400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90800512"/>
+        <c:axId val="75748864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90802048"/>
+        <c:crossAx val="75750400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90802048"/>
+        <c:axId val="75750400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -1132,7 +1152,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90800512"/>
+        <c:crossAx val="75748864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="30"/>
@@ -1146,7 +1166,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1210,7 +1230,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="4.2907152230971107E-2"/>
-                  <c:y val="-2.8351560221638941E-2"/>
+                  <c:y val="-2.8351560221638938E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1234,7 +1254,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="4.1666666666666782E-2"/>
-                  <c:y val="-4.6296296296296424E-3"/>
+                  <c:y val="-4.6296296296296433E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -1262,7 +1282,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-7.8350393700787405E-2"/>
-                  <c:y val="-0.16203703703703737"/>
+                  <c:y val="-0.16203703703703742"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -1276,7 +1296,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-0.13611111111111121"/>
-                  <c:y val="1.8518518518518552E-2"/>
+                  <c:y val="1.8518518518518556E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -1328,19 +1348,19 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>71</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1360,7 +1380,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1377,9 +1397,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.27083333333333326"/>
-          <c:y val="0.11342592592592607"/>
-          <c:w val="0.46388888888889018"/>
-          <c:h val="0.77314814814814958"/>
+          <c:y val="0.11342592592592608"/>
+          <c:w val="0.46388888888889029"/>
+          <c:h val="0.77314814814814981"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -1412,7 +1432,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="3.333333333333334E-2"/>
-                  <c:y val="1.3888888888888926E-2"/>
+                  <c:y val="1.388888888888893E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -1444,7 +1464,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="3.0555555555555582E-2"/>
-                  <c:y val="2.7777777777777891E-2"/>
+                  <c:y val="2.7777777777777901E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -1458,7 +1478,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="3.333333333333334E-2"/>
-                  <c:y val="-9.2592592592593004E-3"/>
+                  <c:y val="-9.2592592592593038E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -1535,7 +1555,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1609,19 +1629,19 @@
                   <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1275</c:v>
+                  <c:v>1325</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3168</c:v>
+                  <c:v>2904</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1845</c:v>
+                  <c:v>1785</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3180</c:v>
+                  <c:v>3390</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1638,7 +1658,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1657,7 +1677,7 @@
           <c:x val="8.1584588656275783E-2"/>
           <c:y val="4.6964973286968567E-2"/>
           <c:w val="0.65982012911893162"/>
-          <c:h val="0.86892327726386565"/>
+          <c:h val="0.86892327726386576"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1765,7 +1785,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>111</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1792,31 +1812,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="107191680"/>
-        <c:axId val="107209856"/>
+        <c:axId val="138334208"/>
+        <c:axId val="138335744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107191680"/>
+        <c:axId val="138334208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="107209856"/>
+        <c:crossAx val="138335744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107209856"/>
+        <c:axId val="138335744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1824,7 +1844,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107191680"/>
+        <c:crossAx val="138334208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1837,7 +1857,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1906,26 +1926,26 @@
                   <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2442</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1200</c:v>
+                  <c:v>1110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="107704704"/>
-        <c:axId val="107706240"/>
+        <c:axId val="75322112"/>
+        <c:axId val="75323648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107704704"/>
+        <c:axId val="75322112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107706240"/>
+        <c:crossAx val="75323648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1933,7 +1953,7 @@
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107706240"/>
+        <c:axId val="75323648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1941,7 +1961,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107704704"/>
+        <c:crossAx val="75322112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="300"/>
@@ -1951,7 +1971,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2041,7 +2061,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2068,7 +2088,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>108</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2095,31 +2115,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>71</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="107811200"/>
-        <c:axId val="107812736"/>
+        <c:axId val="75375360"/>
+        <c:axId val="75376896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107811200"/>
+        <c:axId val="75375360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="107812736"/>
+        <c:crossAx val="75376896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107812736"/>
+        <c:axId val="75376896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2127,19 +2147,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107811200"/>
+        <c:crossAx val="75375360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2150,7 +2171,9 @@
   <c:lang val="it-IT"/>
   <c:style val="7"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2203,29 +2226,29 @@
                   <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>440</c:v>
+                  <c:v>968</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1620</c:v>
+                  <c:v>1560</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1065</c:v>
+                  <c:v>1365</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="107844736"/>
-        <c:axId val="107846272"/>
+        <c:axId val="75412992"/>
+        <c:axId val="75414528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107844736"/>
+        <c:axId val="75412992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107846272"/>
+        <c:crossAx val="75414528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2234,7 +2257,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107846272"/>
+        <c:axId val="75414528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2242,7 +2265,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107844736"/>
+        <c:crossAx val="75412992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="300"/>
@@ -2253,7 +2276,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2403,25 +2426,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="107881216"/>
-        <c:axId val="107882752"/>
+        <c:axId val="75441280"/>
+        <c:axId val="75442816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107881216"/>
+        <c:axId val="75441280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="107882752"/>
+        <c:crossAx val="75442816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107882752"/>
+        <c:axId val="75442816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2429,19 +2452,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107881216"/>
+        <c:crossAx val="75441280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2821,16 +2845,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2851,16 +2875,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3170,7 +3194,7 @@
   <dimension ref="A1:AC41"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="W10" activeCellId="5" sqref="C10 G10 K10 O10 S10 W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3184,41 +3208,41 @@
   <sheetData>
     <row r="1" spans="1:29">
       <c r="A1" s="11"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="14"/>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="14"/>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
       <c r="M1" s="14"/>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
       <c r="Q1" s="14"/>
-      <c r="R1" s="25" t="s">
+      <c r="R1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
       <c r="U1" s="14"/>
-      <c r="V1" s="24" t="s">
+      <c r="V1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
       <c r="Y1" s="9"/>
       <c r="Z1" t="s">
         <v>19</v>
@@ -3320,12 +3344,12 @@
         <v>7</v>
       </c>
       <c r="G3" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="10">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J3" s="5">
         <v>7</v>
@@ -3349,12 +3373,12 @@
         <v>6</v>
       </c>
       <c r="S3" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T3" s="5"/>
       <c r="U3" s="10">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="V3" s="5">
         <v>7</v>
@@ -3367,14 +3391,14 @@
       </c>
       <c r="Z3">
         <f t="shared" ref="Z3:Z7" si="6">SUM(E3,I3,M3,Q3,U3,Y3)</f>
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AA3" s="8">
         <v>25</v>
       </c>
       <c r="AB3">
         <f t="shared" ref="AB3:AB7" si="7">PRODUCT(Z3,AA3)</f>
-        <v>1275</v>
+        <v>1325</v>
       </c>
       <c r="AC3" s="8" t="s">
         <v>1</v>
@@ -3458,10 +3482,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="10">
@@ -3469,9 +3493,11 @@
         <v>23</v>
       </c>
       <c r="F5" s="5">
-        <v>17</v>
-      </c>
-      <c r="G5" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="G5" s="5">
+        <v>6</v>
+      </c>
       <c r="H5" s="5">
         <v>3</v>
       </c>
@@ -3480,16 +3506,16 @@
         <v>20</v>
       </c>
       <c r="J5" s="5">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="10">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N5" s="5">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5">
@@ -3497,13 +3523,13 @@
       </c>
       <c r="Q5" s="10">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="R5" s="5">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="S5" s="5">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="T5" s="5"/>
       <c r="U5" s="10">
@@ -3511,10 +3537,10 @@
         <v>28</v>
       </c>
       <c r="V5" s="5">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="W5" s="5">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="X5" s="5">
         <v>5</v>
@@ -3525,14 +3551,14 @@
       </c>
       <c r="Z5">
         <f t="shared" si="6"/>
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="AA5" s="8">
         <v>22</v>
       </c>
       <c r="AB5">
         <f t="shared" si="7"/>
-        <v>3168</v>
+        <v>2904</v>
       </c>
       <c r="AC5" s="8" t="s">
         <v>3</v>
@@ -3544,23 +3570,23 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="5">
         <v>5</v>
       </c>
       <c r="E6" s="10">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="10">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5">
@@ -3575,12 +3601,12 @@
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="P6" s="5"/>
       <c r="Q6" s="10">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="R6" s="5"/>
       <c r="S6" s="5">
@@ -3595,23 +3621,23 @@
       </c>
       <c r="V6" s="5"/>
       <c r="W6" s="5">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="10">
         <f t="shared" si="4"/>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="Z6">
         <f t="shared" si="6"/>
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="AA6" s="8">
         <v>15</v>
       </c>
       <c r="AB6">
         <f t="shared" si="7"/>
-        <v>1845</v>
+        <v>1785</v>
       </c>
       <c r="AC6" s="8" t="s">
         <v>4</v>
@@ -3622,93 +3648,93 @@
         <v>5</v>
       </c>
       <c r="B7" s="5">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5">
         <v>10</v>
       </c>
       <c r="E7" s="10">
         <f t="shared" si="5"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F7" s="5">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="5">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H7" s="5">
         <v>10</v>
       </c>
       <c r="I7" s="10">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J7" s="5">
         <v>13</v>
       </c>
       <c r="K7" s="5">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="L7" s="5">
         <v>15</v>
       </c>
       <c r="M7" s="10">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="N7" s="5">
         <v>13</v>
       </c>
       <c r="O7" s="5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="P7" s="5">
         <v>13</v>
       </c>
       <c r="Q7" s="10">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="R7" s="5">
+        <v>11</v>
+      </c>
+      <c r="S7" s="5">
         <v>13</v>
-      </c>
-      <c r="S7" s="5">
-        <v>12</v>
       </c>
       <c r="T7" s="5">
         <v>5</v>
       </c>
       <c r="U7" s="10">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V7" s="5">
         <v>13</v>
       </c>
       <c r="W7" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="X7" s="5">
         <v>8</v>
       </c>
       <c r="Y7" s="10">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z7">
         <f t="shared" si="6"/>
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="AA7" s="8">
         <v>15</v>
       </c>
       <c r="AB7">
         <f t="shared" si="7"/>
-        <v>3180</v>
+        <v>3390</v>
       </c>
       <c r="AC7" s="8" t="s">
         <v>5</v>
@@ -3765,7 +3791,7 @@
       </c>
       <c r="AB8" s="15">
         <f>SUM(AB2:AB7)</f>
-        <v>11718</v>
+        <v>11654</v>
       </c>
     </row>
     <row r="9" spans="1:29">
@@ -3842,11 +3868,11 @@
       </c>
       <c r="B10" s="13">
         <f>SUM(B2:B7)</f>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C10" s="13">
         <f>SUM(C2:C7)</f>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D10" s="13">
         <f>SUM(D2:D7)</f>
@@ -3855,11 +3881,11 @@
       <c r="E10" s="9"/>
       <c r="F10" s="13">
         <f t="shared" ref="F10:X10" si="8">SUM(F2:F7)</f>
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" si="8"/>
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="H10" s="13">
         <f t="shared" si="8"/>
@@ -3868,11 +3894,11 @@
       <c r="I10" s="9"/>
       <c r="J10" s="13">
         <f t="shared" si="8"/>
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K10" s="13">
         <f t="shared" si="8"/>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="L10" s="13">
         <f t="shared" si="8"/>
@@ -3881,11 +3907,11 @@
       <c r="M10" s="9"/>
       <c r="N10" s="13">
         <f t="shared" si="8"/>
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="O10" s="13">
         <f t="shared" si="8"/>
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P10" s="13">
         <f t="shared" si="8"/>
@@ -3894,11 +3920,11 @@
       <c r="Q10" s="9"/>
       <c r="R10" s="13">
         <f t="shared" si="8"/>
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="S10" s="13">
         <f t="shared" si="8"/>
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="T10" s="13">
         <f t="shared" si="8"/>
@@ -3907,11 +3933,11 @@
       <c r="U10" s="9"/>
       <c r="V10" s="13">
         <f t="shared" si="8"/>
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="W10" s="13">
         <f t="shared" si="8"/>
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="X10" s="13">
         <f t="shared" si="8"/>
@@ -3923,7 +3949,7 @@
       </c>
       <c r="AB10">
         <f>SUM(AB8-AB9)</f>
-        <v>576</v>
+        <v>512</v>
       </c>
     </row>
     <row r="13" spans="1:29">
@@ -3993,11 +4019,11 @@
       </c>
       <c r="D15">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <f t="shared" ref="E15:E19" si="13">PRODUCT(D15,AA3)</f>
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="F15">
         <f t="shared" si="10"/>
@@ -4043,19 +4069,19 @@
       </c>
       <c r="B17">
         <f t="shared" ref="B17" si="16">SUM(B5,F5,J5,N5,R5,V5)</f>
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="C17" s="8">
         <f t="shared" si="12"/>
-        <v>2442</v>
+        <v>1650</v>
       </c>
       <c r="D17">
         <f t="shared" si="9"/>
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="E17">
         <f t="shared" si="13"/>
-        <v>440</v>
+        <v>968</v>
       </c>
       <c r="F17">
         <f t="shared" si="10"/>
@@ -4082,11 +4108,11 @@
       </c>
       <c r="D18">
         <f t="shared" si="9"/>
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E18">
         <f t="shared" si="13"/>
-        <v>1620</v>
+        <v>1560</v>
       </c>
       <c r="F18">
         <f t="shared" si="10"/>
@@ -4103,19 +4129,19 @@
       </c>
       <c r="B19">
         <f t="shared" ref="B19" si="18">SUM(B7,F7,J7,N7,R7,V7)</f>
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C19" s="8">
         <f t="shared" si="12"/>
-        <v>1200</v>
+        <v>1110</v>
       </c>
       <c r="D19">
         <f t="shared" si="9"/>
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="E19">
         <f t="shared" si="13"/>
-        <v>1065</v>
+        <v>1365</v>
       </c>
       <c r="F19">
         <f t="shared" si="10"/>
@@ -4132,19 +4158,19 @@
       </c>
       <c r="B20">
         <f>SUM(B10,F10,J10,N10,R10,V10)</f>
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="C20" s="8">
         <f>SUM(C14:C19)</f>
-        <v>5417</v>
+        <v>4535</v>
       </c>
       <c r="D20">
         <f>SUM(C10,G10,K10,O10,S10,W10)</f>
-        <v>239</v>
+        <v>281</v>
       </c>
       <c r="E20">
         <f>SUM(E14:E19)</f>
-        <v>4125</v>
+        <v>4943</v>
       </c>
       <c r="F20">
         <f>SUM(D10,H10,L10,P10,T10,X10)</f>
@@ -4157,18 +4183,18 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="17"/>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="23"/>
+      <c r="E22" s="24"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="17"/>
-      <c r="D23" s="23">
+      <c r="D23" s="24">
         <f>SUM(B20,D20,F20)</f>
         <v>620</v>
       </c>
-      <c r="E23" s="23"/>
+      <c r="E23" s="24"/>
     </row>
     <row r="24" spans="1:9">
       <c r="D24" t="s">
@@ -4191,28 +4217,28 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C30">
         <f>B20</f>
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="D30">
         <f>SUM(PRODUCT(B14,AA2),PRODUCT(B15,AA3),PRODUCT(B16,AA4),PRODUCT(B17,AA5),PRODUCT(B18,AA6),PRODUCT(B19,AA7),)</f>
-        <v>5417</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C31">
         <f>D20</f>
-        <v>239</v>
+        <v>281</v>
       </c>
       <c r="D31">
         <f>SUM(PRODUCT(D14,AA2),PRODUCT(D15,AA3),PRODUCT(D16,AA4),PRODUCT(D17,AA5),PRODUCT(D18,AA6),PRODUCT(D19,AA7),)</f>
-        <v>4125</v>
+        <v>4943</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -4235,7 +4261,7 @@
       </c>
       <c r="D33">
         <f>SUM(D30:D32)</f>
-        <v>11718</v>
+        <v>11654</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -4247,7 +4273,13 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="5"/>
+      <c r="A35" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <f>D33-D34</f>
+        <v>209</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="5"/>
@@ -4299,25 +4331,25 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:7">
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="26"/>
+      <c r="F5" s="27"/>
       <c r="G5" t="s">
         <v>33</v>
       </c>
@@ -4504,25 +4536,25 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:7">
       <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26" t="s">
+      <c r="D22" s="27"/>
+      <c r="E22" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="26"/>
+      <c r="F22" s="27"/>
       <c r="G22" t="s">
         <v>33</v>
       </c>
@@ -4592,33 +4624,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:E28"/>
+  <dimension ref="A3:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="B4" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
@@ -4628,10 +4672,23 @@
       <c r="C5" s="5">
         <v>15</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="D5">
+        <f>C5-B5</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>450</v>
+      </c>
+      <c r="F5">
+        <f>C5*30</f>
+        <v>450</v>
+      </c>
+      <c r="G5">
+        <f>F5-E5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
@@ -4641,10 +4698,23 @@
       <c r="C6" s="5">
         <v>41</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="D6">
+        <f t="shared" ref="D6:D11" si="0">C6-B6</f>
+        <v>11</v>
+      </c>
+      <c r="E6" s="5">
+        <v>750</v>
+      </c>
+      <c r="F6">
+        <f>C6*25</f>
+        <v>1025</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G10" si="1">F6-E6</f>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="8" t="s">
         <v>2</v>
       </c>
@@ -4654,10 +4724,23 @@
       <c r="C7" s="5">
         <v>15</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>300</v>
+      </c>
+      <c r="F7">
+        <f>C7*20</f>
+        <v>300</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
@@ -4665,12 +4748,25 @@
         <v>112</v>
       </c>
       <c r="C8" s="5">
-        <v>111</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5">
+        <v>75</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-37</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2464</v>
+      </c>
+      <c r="F8">
+        <f>C8*22</f>
+        <v>1650</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>-814</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
@@ -4680,10 +4776,23 @@
       <c r="C9" s="5">
         <v>0</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>C9*15</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
@@ -4691,12 +4800,25 @@
         <v>89</v>
       </c>
       <c r="C10" s="5">
-        <v>80</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5">
+        <v>74</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-15</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1335</v>
+      </c>
+      <c r="F10">
+        <f>C10*15</f>
+        <v>1110</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>-225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -4704,20 +4826,51 @@
         <v>261</v>
       </c>
       <c r="C11" s="5">
-        <v>262</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="21" spans="1:3">
+        <f>SUM(C5:C10)</f>
+        <v>220</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-41</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5299</v>
+      </c>
+      <c r="F11" s="5">
+        <f>SUM(F5:F10)</f>
+        <v>4535</v>
+      </c>
+      <c r="G11">
+        <f>F11-E11</f>
+        <v>-764</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="B21" t="s">
         <v>34</v>
       </c>
       <c r="C21" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="8" t="s">
         <v>0</v>
       </c>
@@ -4727,8 +4880,24 @@
       <c r="C22">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <f>C22-B22</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f>B22*30</f>
+        <v>450</v>
+      </c>
+      <c r="F22">
+        <f>C22*30</f>
+        <v>450</v>
+      </c>
+      <c r="G22">
+        <f>F22-E22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="8" t="s">
         <v>1</v>
       </c>
@@ -4736,10 +4905,26 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>12</v>
+      </c>
+      <c r="D23">
+        <f>C23-B23</f>
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <f>B23*25</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>C23*25</f>
+        <v>300</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G28" si="2">F23-E23</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="8" t="s">
         <v>2</v>
       </c>
@@ -4749,8 +4934,24 @@
       <c r="C24">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24">
+        <f>C24-B24</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f>B24*20</f>
+        <v>300</v>
+      </c>
+      <c r="F24">
+        <f>C24*20</f>
+        <v>300</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="8" t="s">
         <v>3</v>
       </c>
@@ -4758,10 +4959,26 @@
         <v>25</v>
       </c>
       <c r="C25">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>44</v>
+      </c>
+      <c r="D25">
+        <f>C25-B25</f>
+        <v>19</v>
+      </c>
+      <c r="E25">
+        <f>B25*22</f>
+        <v>550</v>
+      </c>
+      <c r="F25">
+        <f>C25*22</f>
+        <v>968</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="8" t="s">
         <v>4</v>
       </c>
@@ -4769,10 +4986,26 @@
         <v>118</v>
       </c>
       <c r="C26">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>104</v>
+      </c>
+      <c r="D26">
+        <f>C26-B26</f>
+        <v>-14</v>
+      </c>
+      <c r="E26">
+        <f>B26*15</f>
+        <v>1770</v>
+      </c>
+      <c r="F26">
+        <f>C26*15</f>
+        <v>1560</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>-210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="8" t="s">
         <v>5</v>
       </c>
@@ -4780,10 +5013,26 @@
         <v>60</v>
       </c>
       <c r="C27">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>91</v>
+      </c>
+      <c r="D27">
+        <f>C27-B27</f>
+        <v>31</v>
+      </c>
+      <c r="E27">
+        <f>B27*15</f>
+        <v>900</v>
+      </c>
+      <c r="F27">
+        <f>C27*15</f>
+        <v>1365</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>465</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -4791,7 +5040,24 @@
         <v>233</v>
       </c>
       <c r="C28">
-        <v>239</v>
+        <f>SUM(C22:C27)</f>
+        <v>281</v>
+      </c>
+      <c r="D28">
+        <f>C28-B28</f>
+        <v>48</v>
+      </c>
+      <c r="E28">
+        <f>SUM(E22:E27)</f>
+        <v>3970</v>
+      </c>
+      <c r="F28" s="5">
+        <f>SUM(F22:F27)</f>
+        <v>4943</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>973</v>
       </c>
     </row>
   </sheetData>
@@ -4804,8 +5070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4816,41 +5082,41 @@
   <sheetData>
     <row r="1" spans="1:29">
       <c r="A1" s="11"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="14"/>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="14"/>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
       <c r="M1" s="14"/>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
       <c r="Q1" s="14"/>
-      <c r="R1" s="25" t="s">
+      <c r="R1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
       <c r="U1" s="14"/>
-      <c r="V1" s="24" t="s">
+      <c r="V1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
       <c r="Y1" s="9"/>
       <c r="Z1" t="s">
         <v>19</v>
@@ -5780,17 +6046,17 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="23"/>
+      <c r="E22" s="24"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="D23" s="23">
+      <c r="D23" s="24">
         <f>SUM(B20,D20,F20)</f>
         <v>613</v>
       </c>
-      <c r="E23" s="23"/>
+      <c r="E23" s="24"/>
     </row>
     <row r="24" spans="1:7">
       <c r="D24" t="s">

</xml_diff>